<commit_message>
Created a file showing the randomly generated preserves and their probability of survival for both tuna and sharks.
</commit_message>
<xml_diff>
--- a/ESM204_HW1.xlsx
+++ b/ESM204_HW1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/madelinegorchels/Desktop/UCSB/Spring2019/Econ/ESM204Assn1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56DE12C5-BC12-4847-B438-1DA052DB16DE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DED7AE0-E860-A44A-862D-D4D3A21D71DB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15040" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HW1 Data (2)" sheetId="2" r:id="rId1"/>
@@ -969,8 +969,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L485"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -24348,9 +24348,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:O485"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="R4" sqref="R4"/>
+      <selection pane="bottomLeft" activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>